<commit_message>
Updated LP model to include specialty and subspecialty constraints effectively
</commit_message>
<xml_diff>
--- a/PGY2_Allocations_export.xlsx
+++ b/PGY2_Allocations_export.xlsx
@@ -437,12 +437,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 6) (PGY1/2)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -521,12 +521,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Medicine - MACU (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -558,7 +558,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -726,17 +726,17 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ARRH General Medicine (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>JHH Surgery - Vascular (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
         </is>
       </c>
     </row>
@@ -778,7 +778,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -941,12 +941,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>CMN Surgery (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>JHH Acute General Surgery Unit (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -978,12 +978,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1025,12 +1025,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1062,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>JHH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>JHH Surgery - Vascular (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1151,12 +1151,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1193,12 +1193,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
+          <t>JHH Medicine Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>JHH General Surgery / Trauma (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1235,12 +1235,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 6) (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1277,12 +1277,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
+          <t>BDH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
           <t>JHH ICU (PGY2)</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
         </is>
       </c>
     </row>
@@ -1445,12 +1445,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1608,17 +1608,17 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1650,17 +1650,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
           <t>CMN Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1692,12 +1692,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1734,12 +1734,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>CMN Surgery (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1818,12 +1818,12 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1860,17 +1860,17 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
           <t>BDH After Hours Internal Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1949,12 +1949,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
+          <t>MBH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
           <t>MH General Medicine (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2075,12 +2075,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
         </is>
       </c>
     </row>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2159,12 +2159,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2238,17 +2238,17 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2322,17 +2322,17 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2364,17 +2364,17 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>MH KK Rehabilitation (PGY 1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>JHH Forensic Pathology (PGY2)</t>
         </is>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2453,12 +2453,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2490,17 +2490,17 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
           <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Cardiology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2621,12 +2621,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>MH  Medicine - Cardiology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2742,12 +2742,12 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
           <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -2784,7 +2784,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2873,12 +2873,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2910,12 +2910,12 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
           <t>JHH ICU (PGY2)</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2952,17 +2952,17 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2994,17 +2994,17 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
         </is>
       </c>
     </row>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3083,12 +3083,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
           <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
+          <t>MH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
           <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3293,12 +3293,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
           <t>MBH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
           <t>JHH General Paediatrics (PGY2)</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rheumatology (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3456,12 +3456,12 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
+          <t>MBH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
           <t>JHH General Medicine (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
         </is>
       </c>
     </row>
@@ -3592,7 +3592,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>JHH Forensic Pathology (PGY2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3634,7 +3634,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
     </row>
@@ -3666,17 +3666,17 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
+          <t>MH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
           <t>JHH Surgery - Urology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>MH  Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -3750,17 +3750,17 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3792,12 +3792,12 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
+          <t>CMN Palliative Care (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
           <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3881,12 +3881,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatrics (PGY2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3928,7 +3928,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
+          <t>JHH Surgery - Paediatrics (PGY2)</t>
         </is>
       </c>
     </row>
@@ -3960,17 +3960,17 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4044,17 +4044,17 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>MH KK Rehabilitation (PGY 1/2)</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH Medicine - Rheumatology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4212,17 +4212,17 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
           <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4301,12 +4301,12 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4338,7 +4338,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4548,12 +4548,12 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>TRRH Surgery - Orthopaedics 02 (PGY1/2)</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -4637,12 +4637,12 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
+          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
           <t>ARRH Paediatrics (PGY2)</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4721,12 +4721,12 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>JHH Medicine - MACU (PGY1/2)</t>
+          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4758,12 +4758,12 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
           <t>JHH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -4805,12 +4805,12 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
+          <t>JHH Surgery Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
           <t>ARRH General Medicine (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4847,12 +4847,12 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>TRRH Surgery - Orthopaedics 02 (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4884,17 +4884,17 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>BDH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
           <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4968,17 +4968,17 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
     </row>
@@ -5015,12 +5015,12 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>CMN Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>99.09</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>91.82</t>
+          <t>90.91</t>
         </is>
       </c>
     </row>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>69.09</t>
+          <t>57.27</t>
         </is>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>99.09</t>
         </is>
       </c>
     </row>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24.47</t>
+          <t>25.76</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>61.55</t>
+          <t>62.67</t>
         </is>
       </c>
     </row>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1.89</t>
+          <t>2.16</t>
         </is>
       </c>
     </row>
@@ -5141,7 +5141,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27.20</t>
+          <t>27.25</t>
         </is>
       </c>
     </row>
@@ -5228,11 +5228,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 6) (PGY1/2)</t>
         </is>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -5243,11 +5243,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
@@ -5378,11 +5378,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
         </is>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -5393,11 +5393,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Medicine - MACU (PGY1/2)</t>
         </is>
       </c>
       <c r="C16">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17">
@@ -5438,11 +5438,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C19">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20">
@@ -5468,11 +5468,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -5513,11 +5513,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C24">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25">
@@ -5543,11 +5543,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
       <c r="C26">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C29">
-        <v>72</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -5618,11 +5618,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32">
@@ -5693,11 +5693,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C36">
-        <v>72</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37">
@@ -5738,11 +5738,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="C39">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40">
@@ -5753,11 +5753,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C40">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41">
@@ -5768,11 +5768,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C41">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42">
@@ -5843,11 +5843,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47">
@@ -5918,11 +5918,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52">
@@ -5993,11 +5993,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C56">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57">
@@ -6128,11 +6128,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C65">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -6143,11 +6143,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
@@ -6188,11 +6188,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C69">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70">
@@ -6203,11 +6203,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C70">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -6278,11 +6278,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C75">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
@@ -6293,11 +6293,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77">
@@ -6338,11 +6338,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C79">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
@@ -6353,11 +6353,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81">
@@ -6503,11 +6503,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C90">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91">
@@ -6518,11 +6518,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C91">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92">
@@ -6578,11 +6578,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C95">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96">
@@ -6593,11 +6593,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="C96">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="97">
@@ -6653,11 +6653,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 6) (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101">
@@ -6668,11 +6668,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="102">
@@ -6728,11 +6728,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C105">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106">
@@ -6743,11 +6743,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C106">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107">
@@ -6968,11 +6968,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
         </is>
       </c>
       <c r="C121">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="122">
@@ -7028,11 +7028,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C125">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126">
@@ -7043,11 +7043,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
         </is>
       </c>
       <c r="C126">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
@@ -7118,11 +7118,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="C131">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="132">
@@ -7238,11 +7238,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C139">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140">
@@ -7253,11 +7253,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141">
@@ -7268,11 +7268,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C141">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="142">
@@ -7313,11 +7313,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="145">
@@ -7328,11 +7328,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="146">
@@ -7343,11 +7343,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C146">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147">
@@ -7388,11 +7388,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C149">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="150">
@@ -7403,11 +7403,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C150">
-        <v>46</v>
+        <v>69</v>
       </c>
     </row>
     <row r="151">
@@ -7418,11 +7418,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C151">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="152">
@@ -7463,11 +7463,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C154">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="155">
@@ -7478,11 +7478,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
       <c r="C155">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156">
@@ -7538,11 +7538,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C159">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
@@ -7553,11 +7553,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="C160">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161">
@@ -7688,11 +7688,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
       <c r="C169">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170">
@@ -7703,11 +7703,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="C170">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="171">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C174">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="175">
@@ -7778,11 +7778,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C175">
-        <v>77</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
@@ -7793,11 +7793,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C176">
-        <v>3</v>
+        <v>74</v>
       </c>
     </row>
     <row r="177">
@@ -7868,11 +7868,11 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C181">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="182">
@@ -7928,11 +7928,11 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C185">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="186">
@@ -7943,11 +7943,11 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C186">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="187">
@@ -8078,11 +8078,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C195">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="196">
@@ -8153,11 +8153,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C200">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="201">
@@ -8168,11 +8168,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
         </is>
       </c>
       <c r="C201">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="202">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="C204">
-        <v>57</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205">
@@ -8243,11 +8243,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="C206">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="207">
@@ -8303,11 +8303,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C210">
-        <v>77</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211">
@@ -8318,11 +8318,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C211">
-        <v>2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="212">
@@ -8363,11 +8363,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C214">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="215">
@@ -8393,11 +8393,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Colorectal (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C216">
-        <v>2</v>
+        <v>76</v>
       </c>
     </row>
     <row r="217">
@@ -8438,11 +8438,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C219">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220">
@@ -8453,11 +8453,11 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C220">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="221">
@@ -8468,11 +8468,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C221">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="222">
@@ -8513,11 +8513,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="C224">
-        <v>64</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225">
@@ -8543,11 +8543,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C226">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="227">
@@ -8588,11 +8588,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C229">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="230">
@@ -8603,11 +8603,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C230">
-        <v>66</v>
+        <v>17</v>
       </c>
     </row>
     <row r="231">
@@ -8618,11 +8618,11 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C231">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="232">
@@ -8663,11 +8663,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C234">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235">
@@ -8678,11 +8678,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>MH KK Rehabilitation (PGY 1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C235">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
     <row r="236">
@@ -8693,11 +8693,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>JHH Forensic Pathology (PGY2)</t>
         </is>
       </c>
       <c r="C236">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="237">
@@ -8768,11 +8768,11 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
       <c r="C241">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="242">
@@ -8828,11 +8828,11 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C245">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -8843,11 +8843,11 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C246">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="247">
@@ -8888,11 +8888,11 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C249">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="250">
@@ -8903,11 +8903,11 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>CMN Medicine - Cardiology (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C250">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="251">
@@ -8918,11 +8918,11 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C251">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="252">
@@ -8993,11 +8993,11 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C256">
-        <v>30</v>
+        <v>71</v>
       </c>
     </row>
     <row r="257">
@@ -9128,11 +9128,11 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>MH  Medicine - Cardiology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C265">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="266">
@@ -9143,11 +9143,11 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C266">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="267">
@@ -9338,11 +9338,11 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="C279">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="280">
@@ -9353,11 +9353,11 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C280">
-        <v>3</v>
+        <v>76</v>
       </c>
     </row>
     <row r="281">
@@ -9413,11 +9413,11 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="C284">
-        <v>1</v>
+        <v>76</v>
       </c>
     </row>
     <row r="285">
@@ -9443,11 +9443,11 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C286">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="287">
@@ -9518,11 +9518,11 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C291">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="292">
@@ -9578,11 +9578,11 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C295">
-        <v>76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">
@@ -9593,11 +9593,11 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C296">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="297">
@@ -9638,11 +9638,11 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C299">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300">
@@ -9653,11 +9653,11 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C300">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="301">
@@ -9713,11 +9713,11 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>HNE Mental Health Lake Macquarie Ward - Mater hospital (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C304">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="305">
@@ -9728,11 +9728,11 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C305">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="306">
@@ -9743,11 +9743,11 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C306">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="307">
@@ -9788,11 +9788,11 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
+          <t>JHH Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C309">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="310">
@@ -9803,11 +9803,11 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>JHH Medicine - Cardiology (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C310">
-        <v>2</v>
+        <v>53</v>
       </c>
     </row>
     <row r="311">
@@ -9818,11 +9818,11 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
         </is>
       </c>
       <c r="C311">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="312">
@@ -9893,11 +9893,11 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C316">
-        <v>60</v>
+        <v>19</v>
       </c>
     </row>
     <row r="317">
@@ -9953,11 +9953,11 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C320">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="321">
@@ -9968,11 +9968,11 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="C321">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="322">
@@ -10028,11 +10028,11 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C325">
-        <v>77</v>
+        <v>48</v>
       </c>
     </row>
     <row r="326">
@@ -10043,11 +10043,11 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C326">
-        <v>48</v>
+        <v>77</v>
       </c>
     </row>
     <row r="327">
@@ -10193,11 +10193,11 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C336">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="337">
@@ -10268,11 +10268,11 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C341">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="342">
@@ -10328,11 +10328,11 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C345">
-        <v>47</v>
+        <v>3</v>
       </c>
     </row>
     <row r="346">
@@ -10343,11 +10343,11 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C346">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="347">
@@ -10403,11 +10403,11 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C350">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="351">
@@ -10418,11 +10418,11 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C351">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="352">
@@ -10568,11 +10568,11 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rheumatology (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C361">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="362">
@@ -10613,11 +10613,11 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>JHH General Medicine (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C364">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="365">
@@ -10628,11 +10628,11 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>JHH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C365">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="366">
@@ -10793,11 +10793,11 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Mental Health Child Psychiatry (JHH) (PGY2)</t>
         </is>
       </c>
       <c r="C376">
-        <v>73</v>
+        <v>4</v>
       </c>
     </row>
     <row r="377">
@@ -10868,11 +10868,11 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>JHH Forensic Pathology (PGY2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C381">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="382">
@@ -10943,11 +10943,11 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C386">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="387">
@@ -10988,11 +10988,11 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C389">
-        <v>74</v>
+        <v>24</v>
       </c>
     </row>
     <row r="390">
@@ -11018,11 +11018,11 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="C391">
-        <v>24</v>
+        <v>74</v>
       </c>
     </row>
     <row r="392">
@@ -11078,11 +11078,11 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>MH  Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C395">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="396">
@@ -11138,11 +11138,11 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C399">
-        <v>1</v>
+        <v>37</v>
       </c>
     </row>
     <row r="400">
@@ -11153,11 +11153,11 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C400">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="401">
@@ -11168,11 +11168,11 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C401">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="402">
@@ -11213,11 +11213,11 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
       <c r="C404">
-        <v>68</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405">
@@ -11228,11 +11228,11 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C405">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="406">
@@ -11378,11 +11378,11 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C415">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="416">
@@ -11393,11 +11393,11 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatrics (PGY2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C416">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="417">
@@ -11468,11 +11468,11 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
+          <t>JHH Surgery - Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C421">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="422">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C424">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="425">
@@ -11528,11 +11528,11 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="C425">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="426">
@@ -11543,11 +11543,11 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
       <c r="C426">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="427">
@@ -11663,11 +11663,11 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C434">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="435">
@@ -11678,11 +11678,11 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>MH KK Rehabilitation (PGY 1/2)</t>
         </is>
       </c>
       <c r="C435">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="436">
@@ -11693,11 +11693,11 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C436">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="437">
@@ -11768,11 +11768,11 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH Medicine - Rheumatology (PGY1/2)</t>
         </is>
       </c>
       <c r="C441">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="442">
@@ -11843,11 +11843,11 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C446">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="447">
@@ -11963,11 +11963,11 @@
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C454">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="455">
@@ -11978,11 +11978,11 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C455">
-        <v>64</v>
+        <v>34</v>
       </c>
     </row>
     <row r="456">
@@ -11993,11 +11993,11 @@
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C456">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="457">
@@ -12128,11 +12128,11 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C465">
-        <v>65</v>
+        <v>4</v>
       </c>
     </row>
     <row r="466">
@@ -12143,11 +12143,11 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C466">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="467">
@@ -12188,11 +12188,11 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C469">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="470">
@@ -12218,11 +12218,11 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
       <c r="C471">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="472">
@@ -12443,11 +12443,11 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C486">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="487">
@@ -12518,11 +12518,11 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>CMN Medicine - Haematology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C491">
-        <v>75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="492">
@@ -12563,11 +12563,11 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C494">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="495">
@@ -12578,11 +12578,11 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>TRRH Surgery - Orthopaedics 02 (PGY1/2)</t>
         </is>
       </c>
       <c r="C495">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="496">
@@ -12728,11 +12728,11 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
         </is>
       </c>
       <c r="C505">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="506">
@@ -12743,11 +12743,11 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C506">
-        <v>31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="507">
@@ -12878,11 +12878,11 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C515">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="516">
@@ -12893,11 +12893,11 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>JHH Medicine - MACU (PGY1/2)</t>
+          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C516">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="517">
@@ -12938,11 +12938,11 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C519">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="520">
@@ -12953,11 +12953,11 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C520">
-        <v>76</v>
+        <v>5</v>
       </c>
     </row>
     <row r="521">
@@ -13028,11 +13028,11 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C525">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="526">
@@ -13043,11 +13043,11 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C526">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="527">
@@ -13103,11 +13103,11 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>TRRH Surgery - Orthopaedics 02 (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C530">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="531">
@@ -13118,11 +13118,11 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C531">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="532">
@@ -13163,11 +13163,11 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C534">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="535">
@@ -13178,11 +13178,11 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C535">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="536">
@@ -13193,11 +13193,11 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C536">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="537">
@@ -13313,11 +13313,11 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C544">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="545">
@@ -13328,11 +13328,11 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C545">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="546">
@@ -13343,11 +13343,11 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C546">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="547">
@@ -13403,11 +13403,11 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>CMN Medicine - Cardiology (PGY1/2)</t>
         </is>
       </c>
       <c r="C550">
-        <v>51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="551">
@@ -13418,11 +13418,11 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C551">
-        <v>79</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -13478,12 +13478,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>34.4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -13542,12 +13542,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>37.6</t>
+          <t>41.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -13562,7 +13562,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -13574,7 +13574,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>35.2</t>
+          <t>42.6</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -13594,7 +13594,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -13606,7 +13606,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>48.0</t>
+          <t>46.4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>28.6</t>
+          <t>28.4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -13670,7 +13670,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>31.2</t>
+          <t>22.0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -13702,7 +13702,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>34.0</t>
+          <t>36.0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -13734,12 +13734,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>30.8</t>
+          <t>41.6</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -13754,7 +13754,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -13766,12 +13766,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>25.6</t>
+          <t>33.2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -13786,7 +13786,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -13798,7 +13798,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21.6</t>
+          <t>23.0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -13894,7 +13894,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>19.2</t>
+          <t>16.2</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -13926,12 +13926,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>15.6</t>
+          <t>21.8</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -14022,7 +14022,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>36.2</t>
+          <t>24.4</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -14086,12 +14086,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>21.6</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -14101,7 +14101,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -14118,7 +14118,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>35.0</t>
+          <t>29.8</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -14138,7 +14138,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -14214,12 +14214,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>14.0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -14246,12 +14246,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -14278,7 +14278,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12.8</t>
+          <t>16.2</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -14342,12 +14342,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>15.8</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -14374,12 +14374,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>36.4</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -14406,12 +14406,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>54.2</t>
+          <t>56.8</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -14438,7 +14438,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>28.0</t>
+          <t>30.6</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -14534,12 +14534,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>38.8</t>
+          <t>47.2</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -14598,12 +14598,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -14694,7 +14694,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>17.6</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -14726,7 +14726,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>31.0</t>
+          <t>40.0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -14746,7 +14746,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -14758,7 +14758,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23.8</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -14790,12 +14790,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>32.8</t>
+          <t>25.4</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -14822,17 +14822,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>18.6</t>
+          <t>38.0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>FALSE</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>TRUE</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -14854,12 +14854,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16.8</t>
+          <t>10.6</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -14886,7 +14886,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>15.8</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -14918,12 +14918,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>33.2</t>
+          <t>18.8</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -14950,7 +14950,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>11.6</t>
+          <t>11.8</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -14982,7 +14982,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>23.2</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -15014,12 +15014,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -15046,17 +15046,17 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>25.8</t>
+          <t>33.6</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>FALSE</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>TRUE</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -15078,7 +15078,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>17.4</t>
+          <t>25.6</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -15142,12 +15142,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>28.8</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -15270,7 +15270,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>40.2</t>
+          <t>51.8</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -15302,7 +15302,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17.8</t>
+          <t>17.2</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -15334,7 +15334,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>24.2</t>
+          <t>14.4</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -15366,7 +15366,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>17.2</t>
+          <t>16.8</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -15398,12 +15398,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>31.6</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -15430,12 +15430,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>17.4</t>
+          <t>22.2</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -15462,7 +15462,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>24.2</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -15590,7 +15590,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>27.4</t>
+          <t>24.4</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -15600,7 +15600,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -15622,7 +15622,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>31.4</t>
+          <t>29.8</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -15654,7 +15654,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>18.8</t>
+          <t>12.2</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -15674,7 +15674,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -15686,7 +15686,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>39.0</t>
+          <t>39.6</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -15750,17 +15750,17 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>18.2</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
           <t>FALSE</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>TRUE</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -15846,12 +15846,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>29.8</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -15878,7 +15878,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>21.4</t>
+          <t>15.6</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -15910,7 +15910,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>30.2</t>
+          <t>44.2</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -15925,7 +15925,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -15974,7 +15974,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>13.8</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -16006,12 +16006,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>37.0</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -16038,12 +16038,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>46.8</t>
+          <t>33.8</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -16102,7 +16102,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>26.4</t>
+          <t>34.2</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -16122,7 +16122,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -16134,12 +16134,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>26.4</t>
+          <t>27.2</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -16149,7 +16149,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>37.4</t>
+          <t>28.0</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -16230,12 +16230,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>26.2</t>
+          <t>49.8</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -16262,7 +16262,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>12.2</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -16294,12 +16294,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>11.6</t>
+          <t>12.8</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -16422,7 +16422,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>29.4</t>
+          <t>25.6</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -16442,7 +16442,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -16454,7 +16454,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>23.0</t>
+          <t>26.8</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -16474,7 +16474,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -16550,7 +16550,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>15.8</t>
+          <t>22.2</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -16582,7 +16582,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>31.6</t>
+          <t>24.0</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -16614,12 +16614,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>23.4</t>
+          <t>36.8</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -16678,7 +16678,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>27.0</t>
+          <t>21.8</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -16742,7 +16742,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>16.8</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -16762,7 +16762,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -16838,7 +16838,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>43.0</t>
+          <t>37.0</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -16870,12 +16870,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>29.4</t>
+          <t>26.6</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -16934,7 +16934,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>19.0</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -16966,7 +16966,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>37.2</t>
+          <t>18.6</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -44325,7 +44325,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -44352,7 +44352,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -44379,7 +44379,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -44406,7 +44406,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -44433,12 +44433,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>MBH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -44737,12 +44737,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Final clean, algorithm functioning as well as possible.
</commit_message>
<xml_diff>
--- a/PGY2_Allocations_export.xlsx
+++ b/PGY2_Allocations_export.xlsx
@@ -553,7 +553,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
         </is>
       </c>
     </row>
@@ -642,17 +642,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>JHH ICU (PGY2)</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>CMN Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -763,12 +763,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>MBH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -820,7 +820,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -941,12 +941,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>CMN Surgery (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
     </row>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
     </row>
@@ -1309,22 +1309,22 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>JHH ICU (PGY2)</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1351,14 +1351,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>MH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>MH Emergency (PGY1/2)</t>
-        </is>
-      </c>
       <c r="G24" t="inlineStr">
         <is>
           <t>MH General Medicine Relief (PGY2)</t>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>ARRH Surgery - Orthopaedics  (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
           <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1655,12 +1655,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1734,17 +1734,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
-        </is>
-      </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1781,12 +1781,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
           <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -1855,14 +1855,14 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
           <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
       <c r="G36" t="inlineStr">
         <is>
           <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
         </is>
       </c>
     </row>
@@ -1939,12 +1939,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>JHH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
           <t>BDH Surgery (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2070,17 +2070,17 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>CMN Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
-        </is>
-      </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2112,17 +2112,17 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
+          <t>MH General Medicine Relief (PGY2)</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
           <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>HNE Mental Health Newcastle Inpatient Unit - Mater Hospital (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2149,12 +2149,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ARRH General Surgery (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
+          <t>ARRH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2406,17 +2406,17 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
           <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
-        </is>
-      </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2453,12 +2453,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2495,12 +2495,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
     </row>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
     </row>
@@ -2873,12 +2873,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -2910,17 +2910,17 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3083,12 +3083,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
           <t>CMN Relief (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
     </row>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3241,17 +3241,17 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
+          <t>MBH Emergency (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
           <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
+      <c r="G69" t="inlineStr">
         <is>
           <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3330,17 +3330,17 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3414,17 +3414,17 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
           <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>HNE Relief (PGY1/2)</t>
-        </is>
-      </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3498,17 +3498,17 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
+          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
           <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>MH Emergency (PGY1/2)</t>
-        </is>
-      </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+          <t>JHH Medicine - Dermatology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>ARRH Surgery - Orthopaedics  (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -3676,7 +3676,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3797,12 +3797,12 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
         </is>
       </c>
     </row>
@@ -3876,12 +3876,12 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -3928,7 +3928,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatrics (PGY2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4007,7 +4007,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4338,17 +4338,17 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
           <t>JHH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4432,7 +4432,7 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>JHH Medicine - Dermatology (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4585,12 +4585,12 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
+          <t>HNE Relief (PGY1/2)</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
           <t>MH Emergency (PGY1/2)</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -4637,12 +4637,12 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>JHH Surgery - Paediatrics (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4721,12 +4721,12 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4847,12 +4847,12 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
         </is>
       </c>
     </row>
@@ -4889,12 +4889,12 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -4931,12 +4931,12 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
+          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>90.91</t>
+          <t>90.00</t>
         </is>
       </c>
     </row>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>57.27</t>
+          <t>59.09</t>
         </is>
       </c>
     </row>
@@ -5105,7 +5105,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>25.76</t>
+          <t>26.22</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>62.67</t>
+          <t>63.66</t>
         </is>
       </c>
     </row>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2.16</t>
+          <t>2.15</t>
         </is>
       </c>
     </row>
@@ -5141,7 +5141,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>27.25</t>
+          <t>27.88</t>
         </is>
       </c>
     </row>
@@ -5423,11 +5423,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH Surgery Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C18">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
@@ -5543,11 +5543,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
         </is>
       </c>
       <c r="C26">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27">
@@ -5588,11 +5588,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30">
@@ -5603,11 +5603,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C30">
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -5618,11 +5618,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TRRH Emergency (PGY2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C31">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32">
@@ -5693,11 +5693,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
         </is>
       </c>
       <c r="C36">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37">
@@ -5768,11 +5768,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>JHH Surgery - Vascular (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C41">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42">
@@ -5798,11 +5798,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C43">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44">
@@ -5813,11 +5813,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C44">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45">
@@ -5918,11 +5918,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C51">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52">
@@ -5993,11 +5993,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>JHH Medicine - Respiratory (PGY1/2)</t>
+          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
         </is>
       </c>
       <c r="C56">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57">
@@ -6128,11 +6128,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -6143,11 +6143,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67">
@@ -6203,11 +6203,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
+          <t>BDH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C70">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71">
@@ -6293,11 +6293,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C76">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
@@ -6518,11 +6518,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>JHH Medicine Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C91">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92">
@@ -6593,11 +6593,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>JHH General Surgery / Trauma (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C96">
-        <v>44</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97">
@@ -6653,11 +6653,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C100">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="101">
@@ -6713,11 +6713,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C104">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105">
@@ -6743,11 +6743,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C106">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -6773,11 +6773,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C108">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -6788,11 +6788,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C109">
-        <v>66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
@@ -6803,11 +6803,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C110">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111">
@@ -6818,11 +6818,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C111">
-        <v>13</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112">
@@ -6848,11 +6848,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C113">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C114">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -6893,11 +6893,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C116">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="117">
@@ -6968,11 +6968,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C121">
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -7238,11 +7238,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C139">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140">
@@ -7253,11 +7253,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>ARRH Surgery - Orthopaedics  (PGY1/2)</t>
         </is>
       </c>
       <c r="C140">
-        <v>16</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141">
@@ -7268,11 +7268,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C141">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142">
@@ -7403,11 +7403,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C150">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="151">
@@ -7418,11 +7418,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C151">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="152">
@@ -7493,11 +7493,11 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C156">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="157">
@@ -7538,11 +7538,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="C159">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160">
@@ -7553,11 +7553,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C160">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
@@ -7568,11 +7568,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C161">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="162">
@@ -7628,11 +7628,11 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>BDH Acute General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C165">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="166">
@@ -7643,11 +7643,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C166">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="167">
@@ -7748,11 +7748,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C173">
-        <v>5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="174">
@@ -7763,11 +7763,11 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C174">
-        <v>77</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175">
@@ -7793,11 +7793,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
         </is>
       </c>
       <c r="C176">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="177">
@@ -7898,11 +7898,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C183">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -7913,11 +7913,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C184">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185">
@@ -7988,11 +7988,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C189">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="190">
@@ -8018,11 +8018,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C191">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="192">
@@ -8138,11 +8138,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C199">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="200">
@@ -8153,11 +8153,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>BDH After Hours Internal Relief (PGY1/2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C200">
-        <v>79</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -8168,11 +8168,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (Team 3) (PGY2)</t>
+          <t>CMN Palliative Care (PGY1/2)</t>
         </is>
       </c>
       <c r="C201">
-        <v>49</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202">
@@ -8213,11 +8213,11 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="C204">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="205">
@@ -8243,11 +8243,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>JHH Medicine - Nephrology &amp; Dialysis (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="C206">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207">
@@ -8273,11 +8273,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C208">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209">
@@ -8288,11 +8288,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>BDH Surgery (PGY1/2)</t>
+          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
         </is>
       </c>
       <c r="C209">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="210">
@@ -8348,11 +8348,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>ARRH General Surgery (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C213">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214">
@@ -8393,11 +8393,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine - Respiratory (PGY1/2)</t>
         </is>
       </c>
       <c r="C216">
-        <v>76</v>
+        <v>27</v>
       </c>
     </row>
     <row r="217">
@@ -8573,11 +8573,11 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>JHH Surgery Relief (PGY1/2)</t>
+          <t>ARRH General Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C228">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="229">
@@ -8738,11 +8738,11 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C239">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240">
@@ -8753,11 +8753,11 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C240">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241">
@@ -8768,11 +8768,11 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>CMN Palliative Care (PGY1/2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C241">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="242">
@@ -8828,11 +8828,11 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>MH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C245">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="246">
@@ -8843,11 +8843,11 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C246">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="247">
@@ -8903,11 +8903,11 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C250">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="251">
@@ -8918,11 +8918,11 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>JHH Surgery - Neurosurgery (PGY1/2)</t>
+          <t>TRRH Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C251">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="252">
@@ -9068,11 +9068,11 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C261">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="262">
@@ -9443,11 +9443,11 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
         </is>
       </c>
       <c r="C286">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="287">
@@ -9518,11 +9518,11 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="C291">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="292">
@@ -9578,11 +9578,11 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C295">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="296">
@@ -9593,11 +9593,11 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>CMN Emergency (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C296">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="297">
@@ -9638,11 +9638,11 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C299">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300">
@@ -9653,11 +9653,11 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>JHH ICU (PGY2)</t>
+          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
         </is>
       </c>
       <c r="C300">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="301">
@@ -9668,11 +9668,11 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>JHH Medicine Relief (PGY1/2)</t>
+          <t>BDH Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C301">
-        <v>18</v>
+        <v>54</v>
       </c>
     </row>
     <row r="302">
@@ -9818,11 +9818,11 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>JHH Community Acute Post Acute Care Service (PGY2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C311">
-        <v>29</v>
+        <v>77</v>
       </c>
     </row>
     <row r="312">
@@ -9878,11 +9878,11 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="C315">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="316">
@@ -9953,11 +9953,11 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
         </is>
       </c>
       <c r="C320">
-        <v>75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="321">
@@ -9968,11 +9968,11 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>JHH HNELHD Clinical Governance &amp; Indigenous Health Term (PGY2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C321">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="322">
@@ -10043,11 +10043,11 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C326">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="327">
@@ -10193,11 +10193,11 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>CMN Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C336">
-        <v>3</v>
+        <v>54</v>
       </c>
     </row>
     <row r="337">
@@ -10223,11 +10223,11 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C338">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="339">
@@ -10238,11 +10238,11 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
+          <t>CMN Surgery (PGY1/2)</t>
         </is>
       </c>
       <c r="C339">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="340">
@@ -10253,11 +10253,11 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C340">
-        <v>73</v>
+        <v>2</v>
       </c>
     </row>
     <row r="341">
@@ -10388,11 +10388,11 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>JHH General Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C349">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="350">
@@ -10403,11 +10403,11 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C350">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="351">
@@ -10418,11 +10418,11 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>JHH General Paediatrics (PGY2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C351">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="352">
@@ -10493,11 +10493,11 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C356">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="357">
@@ -10538,11 +10538,11 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C359">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="360">
@@ -10553,11 +10553,11 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C360">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="361">
@@ -10568,11 +10568,11 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>CMN Relief (PGY1/2)</t>
+          <t>JHH Surgery - Vascular (PGY1/2)</t>
         </is>
       </c>
       <c r="C361">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="362">
@@ -10688,11 +10688,11 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
         </is>
       </c>
       <c r="C369">
-        <v>77</v>
+        <v>2</v>
       </c>
     </row>
     <row r="370">
@@ -10703,11 +10703,11 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="C370">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="371">
@@ -10718,11 +10718,11 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
+          <t>JHH Medicine - Dermatology (PGY1/2)</t>
         </is>
       </c>
       <c r="C371">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="372">
@@ -10928,11 +10928,11 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>ARRH Surgery - Orthopaedics  (PGY1/2)</t>
+          <t>JHH ICU (PGY2)</t>
         </is>
       </c>
       <c r="C385">
-        <v>72</v>
+        <v>5</v>
       </c>
     </row>
     <row r="386">
@@ -11018,11 +11018,11 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>JHH Surgery - Urology (PGY1/2)</t>
+          <t>JHH General Surgery / Trauma (PGY1/2)</t>
         </is>
       </c>
       <c r="C391">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="392">
@@ -11228,11 +11228,11 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C405">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="406">
@@ -11243,11 +11243,11 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>CMN Medicine - Radiation oncology (01) (PGY2)</t>
         </is>
       </c>
       <c r="C406">
-        <v>26</v>
+        <v>6</v>
       </c>
     </row>
     <row r="407">
@@ -11363,11 +11363,11 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>MH General Medicine (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C414">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="415">
@@ -11378,11 +11378,11 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C415">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="416">
@@ -11468,11 +11468,11 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatrics (PGY2)</t>
+          <t>JHH Surgery - Urology (PGY1/2)</t>
         </is>
       </c>
       <c r="C421">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="422">
@@ -11513,11 +11513,11 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>JHH Medicine - Rehabilitation (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
       <c r="C424">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="425">
@@ -11543,11 +11543,11 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
+          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C426">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="427">
@@ -11573,11 +11573,11 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C428">
-        <v>49</v>
+        <v>4</v>
       </c>
     </row>
     <row r="429">
@@ -11603,11 +11603,11 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Mental Health Older People's Service - Mater Hospital (PGY1/2)</t>
         </is>
       </c>
       <c r="C430">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="431">
@@ -11843,11 +11843,11 @@
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Paediatric Orthopaedics (PGY2)</t>
         </is>
       </c>
       <c r="C446">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="447">
@@ -12143,11 +12143,11 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>CMN Surgery (PGY1/2)</t>
+          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C466">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="467">
@@ -12188,11 +12188,11 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>JHH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C469">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="470">
@@ -12218,11 +12218,11 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>BDH Sub-Acute General Medicine (Team 5) (PGY1/2)</t>
+          <t>JHH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C471">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="472">
@@ -12368,11 +12368,11 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>JHH Medicine - Dermatology (PGY1/2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C481">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="482">
@@ -12443,11 +12443,11 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>CMN Medicine - Medical Oncology (01) (PGY1/2)</t>
+          <t>JHH Acute General Surgery Unit (PGY1/2)</t>
         </is>
       </c>
       <c r="C486">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="487">
@@ -12623,11 +12623,11 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>MH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C498">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="499">
@@ -12638,11 +12638,11 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH Emergency (PGY1/2)</t>
         </is>
       </c>
       <c r="C499">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="500">
@@ -12728,11 +12728,11 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>JHH Medicine - Infectious Disease (PGY1/2)</t>
+          <t>ARRH Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C505">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="506">
@@ -12743,11 +12743,11 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>ARRH Paediatrics (PGY2)</t>
+          <t>JHH Surgery - Paediatrics (PGY2)</t>
         </is>
       </c>
       <c r="C506">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="507">
@@ -12848,11 +12848,11 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>JHH Anaesthetics / Emergency (PGY2)</t>
+          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
         </is>
       </c>
       <c r="C513">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="514">
@@ -12878,11 +12878,11 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>JHH Medicine - Gastroenterology (PGY1/2)</t>
+          <t>BDH After Hours Internal Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="C515">
-        <v>2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="516">
@@ -12893,11 +12893,11 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intermediate Stay - Mater hospital (PGY2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C516">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="517">
@@ -13103,11 +13103,11 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
         </is>
       </c>
       <c r="C530">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="531">
@@ -13118,11 +13118,11 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>HNE Mental Health Intensive Care Unit - Mater hospital (PGY2)</t>
+          <t>JHH Anaesthetics / Emergency (PGY2)</t>
         </is>
       </c>
       <c r="C531">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="532">
@@ -13178,11 +13178,11 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>BDH Emergency (PGY1/2)</t>
+          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
         </is>
       </c>
       <c r="C535">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="536">
@@ -13193,11 +13193,11 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>JHH Surgery - Orthopaedics (PGY1/2)</t>
+          <t>JHH Obstetrics &amp; Gynaecology (PGY1/2)</t>
         </is>
       </c>
       <c r="C536">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="537">
@@ -13253,11 +13253,11 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine (PGY1/2)</t>
+          <t>ARRH General Medicine (PGY1/2)</t>
         </is>
       </c>
       <c r="C540">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="541">
@@ -13268,11 +13268,11 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>BDH Acute General Medicine &amp; Rehabilitation (PGY1/2)</t>
+          <t>CMN Medicine - Gastroenterology with Drug &amp; Alcohol (PGY1/2)</t>
         </is>
       </c>
       <c r="C541">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="542">
@@ -13418,11 +13418,11 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>HNE Mental Health &amp; Substance Use Service - Mater Hospital (PGY1/2)</t>
+          <t>JHH General Surgery / Upper GI (PGY1/2)</t>
         </is>
       </c>
       <c r="C551">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -13574,7 +13574,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>42.6</t>
+          <t>42.4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -13606,7 +13606,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>46.4</t>
+          <t>47.4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>28.4</t>
+          <t>28.6</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -13670,7 +13670,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22.0</t>
+          <t>27.2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -13702,7 +13702,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>36.0</t>
+          <t>30.6</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -13766,7 +13766,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33.2</t>
+          <t>36.8</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -13798,7 +13798,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>23.0</t>
+          <t>28.4</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -13894,7 +13894,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>20.4</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -13926,7 +13926,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21.8</t>
+          <t>16.6</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -14022,7 +14022,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>24.4</t>
+          <t>36.2</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -14054,7 +14054,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>13.4</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -14086,7 +14086,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21.6</t>
+          <t>25.0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -14118,7 +14118,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>29.8</t>
+          <t>31.2</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -14128,7 +14128,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -14138,7 +14138,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -14150,7 +14150,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>18.2</t>
+          <t>17.6</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -14182,7 +14182,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>45.4</t>
+          <t>39.8</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -14192,7 +14192,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -14214,7 +14214,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -14342,7 +14342,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>15.8</t>
+          <t>18.0</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -14406,7 +14406,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>56.8</t>
+          <t>54.6</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -14438,7 +14438,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>30.6</t>
+          <t>38.2</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -14470,7 +14470,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>15.6</t>
+          <t>17.6</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -14480,7 +14480,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -14566,7 +14566,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>32.0</t>
+          <t>26.8</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -14576,7 +14576,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -14662,7 +14662,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>36.2</t>
+          <t>49.6</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -14672,7 +14672,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -14726,7 +14726,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>40.0</t>
+          <t>31.0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -14746,7 +14746,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -14758,7 +14758,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>28.0</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -14790,7 +14790,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>25.4</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -14800,7 +14800,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -14810,7 +14810,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -14822,7 +14822,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>38.0</t>
+          <t>28.0</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -14832,7 +14832,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -14918,7 +14918,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>18.8</t>
+          <t>19.2</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -14928,7 +14928,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -14982,7 +14982,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>23.2</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>30.8</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -15024,7 +15024,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -15046,7 +15046,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>33.6</t>
+          <t>39.6</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -15056,7 +15056,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -15066,7 +15066,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -15110,7 +15110,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>15.8</t>
+          <t>31.2</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -15120,7 +15120,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -15270,7 +15270,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>51.8</t>
+          <t>45.2</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -15290,7 +15290,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -15302,7 +15302,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17.2</t>
+          <t>17.8</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -15334,7 +15334,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>26.6</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -15344,7 +15344,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -15366,7 +15366,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16.8</t>
+          <t>24.4</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -15376,7 +15376,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -15430,7 +15430,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>22.2</t>
+          <t>31.8</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -15462,7 +15462,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>16.8</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -15526,7 +15526,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>41.2</t>
+          <t>39.6</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -15536,7 +15536,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -15590,7 +15590,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>24.4</t>
+          <t>34.6</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -15600,7 +15600,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -15686,7 +15686,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>39.6</t>
+          <t>44.2</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -15696,7 +15696,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -15718,7 +15718,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>32.8</t>
+          <t>31.4</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -15728,7 +15728,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -15750,7 +15750,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>18.2</t>
+          <t>17.0</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -15760,7 +15760,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -15814,7 +15814,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>56.8</t>
+          <t>43.8</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -15910,7 +15910,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>44.2</t>
+          <t>30.8</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -15925,7 +15925,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -15942,7 +15942,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>21.4</t>
+          <t>16.4</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -16038,7 +16038,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>33.8</t>
+          <t>21.4</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -16048,7 +16048,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -16102,7 +16102,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>34.2</t>
+          <t>30.6</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -16122,7 +16122,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -16134,7 +16134,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>27.2</t>
+          <t>29.8</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>28.0</t>
+          <t>40.6</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -16198,7 +16198,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>37.6</t>
+          <t>41.8</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -16208,7 +16208,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -16294,7 +16294,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>12.8</t>
+          <t>18.2</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -16309,7 +16309,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -16422,7 +16422,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>25.6</t>
+          <t>29.4</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -16442,7 +16442,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -16454,7 +16454,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>26.8</t>
+          <t>23.0</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -16474,7 +16474,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>TRUE</t>
+          <t>FALSE</t>
         </is>
       </c>
     </row>
@@ -16518,7 +16518,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>35.6</t>
+          <t>37.0</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -16550,7 +16550,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>22.2</t>
+          <t>15.8</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -16678,7 +16678,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>21.8</t>
+          <t>21.2</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -16742,7 +16742,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>16.8</t>
+          <t>24.6</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -16752,7 +16752,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -16838,7 +16838,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>37.0</t>
+          <t>23.2</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -16848,7 +16848,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -16870,7 +16870,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>26.6</t>
+          <t>19.2</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -16902,7 +16902,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>29.2</t>
+          <t>23.2</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -16922,7 +16922,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>FALSE</t>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -16966,7 +16966,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>18.6</t>
+          <t>29.8</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -44308,7 +44308,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>MBH Emergency (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -44325,7 +44325,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -44335,7 +44335,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -44362,7 +44362,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -44384,12 +44384,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>CMN Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
     </row>
@@ -44411,7 +44411,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ARRH General Medicine (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -44438,7 +44438,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MBH Emergency (PGY1/2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -44725,7 +44725,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>HNE Relief (PGY1/2)</t>
+          <t>MH General Medicine Relief (PGY2)</t>
         </is>
       </c>
     </row>
@@ -44737,7 +44737,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MH General Medicine Relief (PGY2)</t>
+          <t>HNE Relief (PGY1/2)</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">

</xml_diff>